<commit_message>
Prog-entera: Modifica datos problema 11.
</commit_message>
<xml_diff>
--- a/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
+++ b/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
@@ -10,7 +10,7 @@
   <sheets>
     <sheet name="Origenes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Destinos" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Costos-de-Alquiler" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Costos-Capacidades" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Demandas" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
   <si>
     <t xml:space="preserve">Indice</t>
   </si>
@@ -109,7 +109,10 @@
     <t xml:space="preserve">Vinces</t>
   </si>
   <si>
-    <t xml:space="preserve">Costo de Alquiler (USD)</t>
+    <t xml:space="preserve">Costo (USD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Capacidad</t>
   </si>
   <si>
     <t xml:space="preserve">Demanda</t>
@@ -260,11 +263,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -434,11 +437,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +735,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -740,11 +743,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8367346938776"/>
+    <col collapsed="false" hidden="false" max="1022" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -757,6 +761,9 @@
       <c r="C1" s="3" t="s">
         <v>28</v>
       </c>
+      <c r="D1" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -766,6 +773,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="7"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -775,6 +783,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="7"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -784,6 +793,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="7"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -793,6 +803,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="7"/>
+      <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -802,6 +813,7 @@
         <v>8</v>
       </c>
       <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -811,6 +823,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="7"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -820,6 +833,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="7"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -829,6 +843,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="7"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -838,6 +853,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="7"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -847,6 +863,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="7"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -856,6 +873,7 @@
         <v>14</v>
       </c>
       <c r="C12" s="7"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -865,6 +883,7 @@
         <v>15</v>
       </c>
       <c r="C13" s="7"/>
+      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -890,11 +909,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.2857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Prog-entera: Completa datos del problema 11.
</commit_message>
<xml_diff>
--- a/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
+++ b/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Origenes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Destinos" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Costos-Capacidades" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Demandas" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Otros-parametros" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
   <si>
     <t xml:space="preserve">Indice</t>
   </si>
@@ -109,13 +110,37 @@
     <t xml:space="preserve">Vinces</t>
   </si>
   <si>
-    <t xml:space="preserve">Costo (USD)</t>
+    <t xml:space="preserve">Costo (USD/m2)</t>
   </si>
   <si>
     <t xml:space="preserve">Capacidad</t>
   </si>
   <si>
     <t xml:space="preserve">Demanda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parametro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unidades</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area Fija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Area por Estacionamiento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presupuesto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USD</t>
   </si>
 </sst>
 </file>
@@ -205,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,11 +256,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -257,17 +294,17 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -437,11 +474,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -743,12 +780,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="15.8367346938776"/>
-    <col collapsed="false" hidden="false" max="1022" min="5" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="1020" min="5" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,8 +809,12 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="8" t="n">
+        <v>533.82</v>
+      </c>
+      <c r="D2" s="9" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -782,8 +823,12 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="4"/>
+      <c r="C3" s="8" t="n">
+        <v>180.23</v>
+      </c>
+      <c r="D3" s="9" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -792,8 +837,12 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="8" t="n">
+        <v>455.65</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -802,8 +851,12 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="8" t="n">
+        <v>464.15</v>
+      </c>
+      <c r="D5" s="9" t="n">
+        <v>60</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -812,8 +865,12 @@
       <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="8" t="n">
+        <v>557.34</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -822,8 +879,12 @@
       <c r="B7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="8" t="n">
+        <v>515.08</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>49</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -832,8 +893,12 @@
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="8" t="n">
+        <v>286.82</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>59</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -842,8 +907,12 @@
       <c r="B9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="4"/>
+      <c r="C9" s="8" t="n">
+        <v>244.48</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -852,8 +921,12 @@
       <c r="B10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="8" t="n">
+        <v>497.22</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>61</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -862,8 +935,12 @@
       <c r="B11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="8" t="n">
+        <v>572.32</v>
+      </c>
+      <c r="D11" s="9" t="n">
+        <v>51</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -872,8 +949,12 @@
       <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="8" t="n">
+        <v>162.46</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>36</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -882,8 +963,12 @@
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="8" t="n">
+        <v>249.07</v>
+      </c>
+      <c r="D13" s="9" t="n">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -903,17 +988,17 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.8826530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1021" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.96428571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +1019,9 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="10" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="n">
@@ -943,7 +1030,9 @@
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="10" t="n">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
@@ -952,7 +1041,9 @@
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C4" s="10" t="n">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
@@ -961,7 +1052,9 @@
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5"/>
+      <c r="C5" s="10" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -970,7 +1063,9 @@
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="10" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
@@ -979,7 +1074,9 @@
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="10" t="n">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
@@ -988,7 +1085,9 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
+      <c r="C8" s="10" t="n">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
@@ -997,7 +1096,9 @@
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="5"/>
+      <c r="C9" s="10" t="n">
+        <v>27</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
@@ -1006,7 +1107,9 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="5"/>
+      <c r="C10" s="10" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
@@ -1015,7 +1118,9 @@
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="10" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
@@ -1024,7 +1129,9 @@
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="5"/>
+      <c r="C12" s="10" t="n">
+        <v>34</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
@@ -1033,7 +1140,9 @@
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="10" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="n">
@@ -1042,7 +1151,9 @@
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="5"/>
+      <c r="C14" s="10" t="n">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="n">
@@ -1051,7 +1162,9 @@
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="5"/>
+      <c r="C15" s="10" t="n">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="n">
@@ -1060,7 +1173,9 @@
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="5"/>
+      <c r="C16" s="10" t="n">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="n">
@@ -1069,7 +1184,9 @@
       <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="5"/>
+      <c r="C17" s="10" t="n">
+        <v>24</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="n">
@@ -1078,7 +1195,9 @@
       <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="5"/>
+      <c r="C18" s="10" t="n">
+        <v>22</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="n">
@@ -1087,7 +1206,9 @@
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="5"/>
+      <c r="C19" s="10" t="n">
+        <v>23</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="n">
@@ -1096,7 +1217,9 @@
       <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="10" t="n">
+        <v>20</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="n">
@@ -1105,7 +1228,9 @@
       <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="10" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="n">
@@ -1114,7 +1239,9 @@
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="5"/>
+      <c r="C22" s="10" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
@@ -1123,7 +1250,9 @@
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="10" t="n">
+        <v>17</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="n">
@@ -1132,7 +1261,9 @@
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="5"/>
+      <c r="C24" s="10" t="n">
+        <v>14</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="n">
@@ -1141,7 +1272,81 @@
       <c r="B25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="5"/>
+      <c r="C25" s="10" t="n">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="27.780612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>200</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>2400000</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Prog-entera: Modifica datos del problema 11.
</commit_message>
<xml_diff>
--- a/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
+++ b/programacion-entera/codigos/Datos/Datos_Problema-11.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Origenes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Destinos" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Costos-Capacidades" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Costos" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Demandas" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Otros-parametros" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t xml:space="preserve">Indice</t>
   </si>
@@ -113,9 +113,6 @@
     <t xml:space="preserve">Costo (USD/m2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacidad</t>
-  </si>
-  <si>
     <t xml:space="preserve">Demanda</t>
   </si>
   <si>
@@ -137,10 +134,16 @@
     <t xml:space="preserve">Area por Estacionamiento</t>
   </si>
   <si>
-    <t xml:space="preserve">Presupuesto</t>
+    <t xml:space="preserve">Presupuesto 01</t>
   </si>
   <si>
     <t xml:space="preserve">USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presupuesto 02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presupuesto 03</t>
   </si>
 </sst>
 </file>
@@ -230,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,15 +262,11 @@
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,17 +293,17 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -474,11 +473,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1022" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1023" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -772,7 +771,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -780,12 +779,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="19.1683673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="1020" min="5" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1021" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="6" width="18.8979591836735"/>
+    <col collapsed="false" hidden="false" max="1019" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1020" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -798,9 +796,6 @@
       <c r="C1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="n">
@@ -809,11 +804,8 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="8" t="n">
+      <c r="C2" s="7" t="n">
         <v>533.82</v>
-      </c>
-      <c r="D2" s="9" t="n">
-        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -823,11 +815,8 @@
       <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="n">
+      <c r="C3" s="7" t="n">
         <v>180.23</v>
-      </c>
-      <c r="D3" s="9" t="n">
-        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -837,11 +826,8 @@
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="8" t="n">
+      <c r="C4" s="7" t="n">
         <v>455.65</v>
-      </c>
-      <c r="D4" s="9" t="n">
-        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -851,11 +837,8 @@
       <c r="B5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8" t="n">
+      <c r="C5" s="7" t="n">
         <v>464.15</v>
-      </c>
-      <c r="D5" s="9" t="n">
-        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -863,13 +846,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v>557.34</v>
-      </c>
-      <c r="D6" s="9" t="n">
-        <v>39</v>
+        <v>22</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>162.46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -877,13 +857,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="8" t="n">
-        <v>515.08</v>
-      </c>
-      <c r="D7" s="9" t="n">
-        <v>49</v>
+        <v>8</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>557.34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -891,13 +868,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="8" t="n">
-        <v>286.82</v>
-      </c>
-      <c r="D8" s="9" t="n">
-        <v>59</v>
+        <v>9</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>515.08</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -905,13 +879,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="8" t="n">
-        <v>244.48</v>
-      </c>
-      <c r="D9" s="9" t="n">
-        <v>62</v>
+        <v>10</v>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>286.82</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -919,13 +890,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="8" t="n">
-        <v>497.22</v>
-      </c>
-      <c r="D10" s="9" t="n">
-        <v>61</v>
+        <v>11</v>
+      </c>
+      <c r="C10" s="7" t="n">
+        <v>244.48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,13 +901,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="8" t="n">
-        <v>572.32</v>
-      </c>
-      <c r="D11" s="9" t="n">
-        <v>51</v>
+        <v>12</v>
+      </c>
+      <c r="C11" s="7" t="n">
+        <v>497.22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -947,13 +912,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="8" t="n">
-        <v>162.46</v>
-      </c>
-      <c r="D12" s="9" t="n">
-        <v>36</v>
+        <v>13</v>
+      </c>
+      <c r="C12" s="7" t="n">
+        <v>572.32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -963,11 +925,8 @@
       <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="8" t="n">
+      <c r="C13" s="7" t="n">
         <v>249.07</v>
-      </c>
-      <c r="D13" s="9" t="n">
-        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -994,11 +953,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="33.4795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1021" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="32.9387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1021" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="1022" style="0" width="7.83163265306122"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1009,7 +968,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1019,7 +978,7 @@
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="9" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1030,7 +989,7 @@
       <c r="B3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="9" t="n">
         <v>30</v>
       </c>
     </row>
@@ -1041,7 +1000,7 @@
       <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="9" t="n">
         <v>21</v>
       </c>
     </row>
@@ -1052,7 +1011,7 @@
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="9" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1063,7 +1022,7 @@
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="9" t="n">
         <v>28</v>
       </c>
     </row>
@@ -1074,7 +1033,7 @@
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="9" t="n">
         <v>18</v>
       </c>
     </row>
@@ -1085,7 +1044,7 @@
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="9" t="n">
         <v>28</v>
       </c>
     </row>
@@ -1096,7 +1055,7 @@
       <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="9" t="n">
         <v>27</v>
       </c>
     </row>
@@ -1107,7 +1066,7 @@
       <c r="B10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="9" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1118,7 +1077,7 @@
       <c r="B11" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="9" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1129,7 +1088,7 @@
       <c r="B12" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="9" t="n">
         <v>34</v>
       </c>
     </row>
@@ -1140,7 +1099,7 @@
       <c r="B13" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="9" t="n">
         <v>17</v>
       </c>
     </row>
@@ -1151,7 +1110,7 @@
       <c r="B14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="9" t="n">
         <v>16</v>
       </c>
     </row>
@@ -1162,7 +1121,7 @@
       <c r="B15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="9" t="n">
         <v>29</v>
       </c>
     </row>
@@ -1173,7 +1132,7 @@
       <c r="B16" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="9" t="n">
         <v>10</v>
       </c>
     </row>
@@ -1184,7 +1143,7 @@
       <c r="B17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="9" t="n">
         <v>24</v>
       </c>
     </row>
@@ -1195,7 +1154,7 @@
       <c r="B18" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="9" t="n">
         <v>22</v>
       </c>
     </row>
@@ -1206,7 +1165,7 @@
       <c r="B19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="9" t="n">
         <v>23</v>
       </c>
     </row>
@@ -1217,7 +1176,7 @@
       <c r="B20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="9" t="n">
         <v>20</v>
       </c>
     </row>
@@ -1228,7 +1187,7 @@
       <c r="B21" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="9" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1239,7 +1198,7 @@
       <c r="B22" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="9" t="n">
         <v>6</v>
       </c>
     </row>
@@ -1250,7 +1209,7 @@
       <c r="B23" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="9" t="n">
         <v>17</v>
       </c>
     </row>
@@ -1261,7 +1220,7 @@
       <c r="B24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="9" t="n">
         <v>14</v>
       </c>
     </row>
@@ -1272,7 +1231,7 @@
       <c r="B25" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="9" t="n">
         <v>13</v>
       </c>
     </row>
@@ -1292,60 +1251,82 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="27.780612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="27.4030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>220</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>200</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>15</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4" t="n">
+        <v>2500000</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="4" t="n">
-        <v>2400000</v>
-      </c>
-      <c r="C4" s="4" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
         <v>38</v>
+      </c>
+      <c r="B5" s="4" t="n">
+        <v>5000000</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>